<commit_message>
started to generate different designs (size of mxu matrix)
</commit_message>
<xml_diff>
--- a/dtpu_configurations/only_integer8/mxu_8x8_30mhz/timing.xlsx
+++ b/dtpu_configurations/only_integer8/mxu_8x8_30mhz/timing.xlsx
@@ -119,10 +119,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="n" s="4">
-        <v>16.003976821899414</v>
+        <v>13.65286922454834</v>
       </c>
       <c r="C2" t="n" s="4">
-        <v>0.02456146478652954</v>
+        <v>0.007553291507065296</v>
       </c>
     </row>
   </sheetData>

</xml_diff>